<commit_message>
Added bar plot for readme
</commit_message>
<xml_diff>
--- a/Snapshot Figures and Analysis.xlsx
+++ b/Snapshot Figures and Analysis.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Data Scientists/Analysts</t>
   </si>
@@ -56,18 +56,6 @@
   </si>
   <si>
     <t>Bachelors Degrees - Completed and Inbound</t>
-  </si>
-  <si>
-    <t>ANALYSIS</t>
-  </si>
-  <si>
-    <t>Forkaia looks for talents that are well educated given the high number of Degrees and also talents that have specialized in their different fields.</t>
-  </si>
-  <si>
-    <t>Forkaia members are well versed technologically and well educated in their fields.</t>
-  </si>
-  <si>
-    <t>Forkaia believes in using data to guide the future, given the high number of people with knowledge in data science/analytics</t>
   </si>
 </sst>
 </file>
@@ -126,7 +114,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -135,9 +123,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -150,6 +135,257 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Forkaia Talent Showcase</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Count</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$2:$A$13</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>Data Scientists/Analysts</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Bachelors Degrees - Completed and Inbound</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Masters Degrees</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Web/Graphic Designers</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Marketers - Social media, Ads etc.</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Computer Scientists</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Special Awards/Recognition/Honors</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Software Devs/Engineers</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>PhDs and Doctorates</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Web Developers</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Hackathon Champions</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Coding competition winners</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$2:$B$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>2387</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2219</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>561</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>410</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>386</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>309</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>118</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>111</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="151874176"/>
+        <c:axId val="151900928"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="151874176"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="151900928"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="151900928"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="151874176"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>542925</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -439,10 +675,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B23"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="S8" sqref="S8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -468,26 +704,26 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="B3">
-        <v>309</v>
+        <v>2219</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B4">
-        <v>111</v>
+        <v>561</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B5">
-        <v>4</v>
+        <v>410</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -500,26 +736,26 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B7">
-        <v>410</v>
+        <v>309</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B8">
-        <v>2219</v>
+        <v>118</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B9">
-        <v>561</v>
+        <v>111</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -532,62 +768,34 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B11">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B12">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B13">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="22" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="23" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="A23:XFD23"/>
-    <mergeCell ref="A17:XFD17"/>
-    <mergeCell ref="A18:XFD18"/>
-    <mergeCell ref="A19:XFD19"/>
-    <mergeCell ref="A20:XFD20"/>
-    <mergeCell ref="A21:XFD21"/>
-    <mergeCell ref="A22:XFD22"/>
-  </mergeCells>
+  <sortState ref="A2:B13">
+    <sortCondition descending="1" ref="B2:B13"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Labelled axis on image
</commit_message>
<xml_diff>
--- a/Snapshot Figures and Analysis.xlsx
+++ b/Snapshot Figures and Analysis.xlsx
@@ -291,11 +291,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="151874176"/>
-        <c:axId val="151900928"/>
+        <c:axId val="214350464"/>
+        <c:axId val="214352640"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="151874176"/>
+        <c:axId val="214350464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -308,7 +308,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="151900928"/>
+        <c:crossAx val="214352640"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -316,7 +316,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="151900928"/>
+        <c:axId val="214352640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -324,6 +324,21 @@
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Number of people</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
           <c:layout/>
           <c:overlay val="0"/>
         </c:title>
@@ -331,7 +346,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="151874176"/>
+        <c:crossAx val="214350464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -678,7 +693,7 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S8" sqref="S8"/>
+      <selection activeCell="S21" sqref="S21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>